<commit_message>
add flowchart to images folder
</commit_message>
<xml_diff>
--- a/data/Tract.xlsx
+++ b/data/Tract.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/yu_wang_1_vanderbilt_edu/Documents/code/Infrastructure-network-simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/yu_wang_1_vanderbilt_edu/Documents/code/Infrastructure-network-simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="222" documentId="8_{75E77A1A-45B0-42F7-89BE-3D0EC92268AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0497774-D426-44A7-81F3-67AB5346BBAA}"/>
   <bookViews>
-    <workbookView xWindow="14475" yWindow="2850" windowWidth="9045" windowHeight="9285" xr2:uid="{A2C9DC05-224A-4F94-B1F0-33C907EA17A7}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2C9DC05-224A-4F94-B1F0-33C907EA17A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,12 +411,12 @@
   <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -456,7 +456,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -476,7 +476,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>101.1</v>
       </c>
@@ -496,7 +496,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>101.2</v>
       </c>
@@ -517,7 +517,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>102.1</v>
       </c>
@@ -537,7 +537,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>102.2</v>
       </c>
@@ -557,7 +557,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>103</v>
       </c>
@@ -577,7 +577,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>105</v>
       </c>
@@ -597,7 +597,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>106.1</v>
       </c>
@@ -617,7 +617,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>106.2</v>
       </c>
@@ -637,7 +637,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>106.3</v>
       </c>
@@ -657,7 +657,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>107.1</v>
       </c>
@@ -677,7 +677,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>107.2</v>
       </c>
@@ -697,7 +697,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>108.1</v>
       </c>
@@ -717,7 +717,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>108.2</v>
       </c>
@@ -737,7 +737,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>11</v>
       </c>
@@ -757,7 +757,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>110.1</v>
       </c>
@@ -777,7 +777,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>110.2</v>
       </c>
@@ -797,7 +797,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>111</v>
       </c>
@@ -817,7 +817,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>112</v>
       </c>
@@ -837,7 +837,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>113</v>
       </c>
@@ -857,7 +857,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>114</v>
       </c>
@@ -877,7 +877,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>115</v>
       </c>
@@ -897,7 +897,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>116</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>117</v>
       </c>
@@ -937,7 +937,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>118</v>
       </c>
@@ -957,7 +957,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>12</v>
       </c>
@@ -977,7 +977,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>13</v>
       </c>
@@ -997,7 +997,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>14</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>15</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>17</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>19</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>20</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>201.01</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>66.180000000000007</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>201.02</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>28.99</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>202.1</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>202.21</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>20.11</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>202.22</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>13.44</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>203</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>5.96</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>204</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>205.11</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>205.12</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>205.21</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>205.23</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>205.24</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>205.31</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>6.79</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>205.32</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>205.41</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>205.42</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>206.1</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>206.21</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>206.22</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>206.32</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>206.33</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>206.34</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>206.35</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>206.42</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>206.43</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>206.44</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>206.51</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>206.52</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>207</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>208.1</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>43.67</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>208.2</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>27.72</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>208.31</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>208.32</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>9.66</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>209</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>11.21</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>21</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>210.1</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>22.36</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>210.2</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>25.41</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>211.11</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>211.12</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>2.09</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>211.13</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>211.21</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>211.22</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>211.24</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>211.25</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>211.26</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>211.35</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>211.36</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>211.37</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>211.38</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>211.39</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>211.4</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>211.41</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>211.42</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>212</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>213.11</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>213.12</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>213.2</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>213.31</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>213.33</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>213.34</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>213.41</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>213.42</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>213.51</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>213.52</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>213.53</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>6.31</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>214.1</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>214.2</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>214.3</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>215.1</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>215.2</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>18.77</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>215.3</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>215.4</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>7.17</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>216.11</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>216.12</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>216.13</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>216.2</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>217.1</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>217.21</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>217.24</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>217.25</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>217.26</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>217.31</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>217.32</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>217.41</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>217.44</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>217.45</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>217.46</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>217.47</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>217.51</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>217.52</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>217.53</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>217.54</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>219</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>220.22</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>220.23</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>220.24</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>221.11</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>221.12</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>221.21</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>221.22</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>221.3</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>222.1</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>7.96</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>222.2</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>223.1</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>223.21</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>223.22</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>223.3</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>224.1</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>5.21</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>225</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>226</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>15.58</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>227</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>24</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>25</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>26</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>27</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>28</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>29</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>3</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>30</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>31</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>32</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>33</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>34</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>35</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>36</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>37</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>38</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>39</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>4</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>42</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>43</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>45</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>46</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>50</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>53</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>55</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>56</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>57</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>58</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>59</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>6</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>60</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>62</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>63</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>64</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>65</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>66</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>67</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>68</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>69</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>7</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>70</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>71</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>72</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>73</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>74</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>75</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>78.099999999999994</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>78.209999999999994</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>78.22</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>79</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>8</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>80</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>81.099999999999994</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>81.2</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>82</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>85</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>86</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>87</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>88</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>89</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>9</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>91</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>92</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>93</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>94</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>95</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>96</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>97</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>98</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>9801</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>7.39</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>9802</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>17.57</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>9803</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>39.58</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>9804</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>7.04</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>99.01</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>7.36</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>99.02</v>
       </c>
@@ -5048,18 +5048,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5081,18 +5081,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02CCA377-66A8-4AAD-8A62-CA789AF5873F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3F750C-6381-4DFA-BDAD-C2398039F659}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02CCA377-66A8-4AAD-8A62-CA789AF5873F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>